<commit_message>
Version 0.9.1 GUI doesn't work yet
</commit_message>
<xml_diff>
--- a/devices.xlsx
+++ b/devices.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FB9D2F-133F-4A92-BFB1-775A00EB6F54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="5" sheetId="1" r:id="rId1"/>
+    <sheet name="3" sheetId="2" r:id="rId1"/>
+    <sheet name="4" sheetId="3" r:id="rId2"/>
+    <sheet name="5" sheetId="1" r:id="rId3"/>
+    <sheet name="6" sheetId="4" r:id="rId4"/>
+    <sheet name="28" sheetId="5" r:id="rId5"/>
+    <sheet name="70" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -54,9 +60,6 @@
     <t>InfiLINK 2x2 PRO</t>
   </si>
   <si>
-    <t>InfiLINK XG</t>
-  </si>
-  <si>
     <t>Quanta 5</t>
   </si>
   <si>
@@ -68,11 +71,14 @@
   <si>
     <t>R5000-Mmx/5.300.2x500.2x26</t>
   </si>
+  <si>
+    <t>InfiLINK XG 500</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -471,11 +477,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72BA4B9B-0089-40E7-A054-D81F384FF206}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{520D10D5-5FD3-47C1-A520-25C3FFA70CB5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +519,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>2</v>
@@ -1625,7 +1655,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>2</v>
@@ -2876,7 +2906,7 @@
         <v>9</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C58" s="20" t="s">
         <v>2</v>
@@ -2901,7 +2931,7 @@
         <v>0</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C59" s="20"/>
       <c r="D59" s="20"/>
@@ -4010,7 +4040,7 @@
         <v>9</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C82" s="20" t="s">
         <v>2</v>
@@ -4035,7 +4065,7 @@
         <v>0</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C83" s="20"/>
       <c r="D83" s="20"/>
@@ -4619,7 +4649,7 @@
         <v>0</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C98" s="20"/>
       <c r="D98" s="20"/>
@@ -5266,4 +5296,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F441127-AE62-4EEC-9688-913EC40B29FD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE284738-7BB5-4E54-8A16-60E87683C139}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F90EB4-E42E-45D2-A7A7-99502C6DBF64}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>